<commit_message>
Weitere Daten zu Gehäuseinformationen hinzugefügt
</commit_message>
<xml_diff>
--- a/documents/Grundsatzüberlegungen Gehäuse für DiverMarker und Diverflasher.xlsx
+++ b/documents/Grundsatzüberlegungen Gehäuse für DiverMarker und Diverflasher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_Workspaces\diver_led_tools\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC92E2BB-C2C6-4791-82AC-6655325465ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D45A10-D438-4FA6-A51F-3CCCC8841BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3530" yWindow="2630" windowWidth="19620" windowHeight="11400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3530" yWindow="110" windowWidth="19620" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grundmaße" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
-  <si>
-    <t>Grundsätzliche Daten</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Diver Flasher</t>
   </si>
@@ -160,6 +157,18 @@
   </si>
   <si>
     <t>1) ggf Versandkosten sparen, indem alles im Riggatec Shop gekauft wird</t>
+  </si>
+  <si>
+    <t>Grundsätzliche Daten PCB</t>
+  </si>
+  <si>
+    <t>Vorteile ALU</t>
+  </si>
+  <si>
+    <t>Versandkosten 4,90€ pro Bestellung</t>
+  </si>
+  <si>
+    <t>Lieferant GWT für PVC</t>
   </si>
 </sst>
 </file>
@@ -610,7 +619,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,7 +632,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -632,16 +641,16 @@
     <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3"/>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>105</v>
@@ -653,7 +662,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>24</v>
@@ -665,7 +674,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
@@ -677,7 +686,7 @@
     </row>
     <row r="7" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5">
         <v>31</v>
@@ -689,7 +698,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -697,7 +706,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -715,15 +724,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7FDCF4-0073-4686-819C-987F0208FEA8}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
     <col min="2" max="2" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.90625" style="1"/>
@@ -738,7 +747,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -752,48 +761,48 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>32</v>
@@ -809,24 +818,24 @@
         <v>12.99</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -842,24 +851,24 @@
         <v>14.99</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -875,24 +884,24 @@
         <v>13.95</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>36</v>
@@ -908,24 +917,24 @@
         <v>15.75</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>30</v>
@@ -943,24 +952,24 @@
         <v>6.9</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
         <v>35</v>
@@ -978,24 +987,24 @@
         <v>6.9</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1">
         <v>40</v>
@@ -1007,23 +1016,39 @@
         <v>0</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1039,6 +1064,7 @@
     <hyperlink ref="H8" r:id="rId5" xr:uid="{83E8C77D-3B6D-45D1-B2CF-D4ED3A5DD20F}"/>
     <hyperlink ref="H9" r:id="rId6" xr:uid="{9396A90D-7785-4AA5-B375-693E848A3674}"/>
     <hyperlink ref="H11" r:id="rId7" xr:uid="{A0350FA8-3D2D-40F6-888A-D9CBD78819B8}"/>
+    <hyperlink ref="H20" r:id="rId8" xr:uid="{B1EF4879-2600-4758-88BC-CC84F0BFF87B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>